<commit_message>
A bunch of TESTED hot garbage coming through!
</commit_message>
<xml_diff>
--- a/CEDAS.xlsx
+++ b/CEDAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianot\IdeaProjects\enginair-server-side-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F24E6F4-B843-4050-A79D-84D693A5B115}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0673BA-37A4-45C2-A0DF-FEDC2E425DBF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33375" yWindow="2505" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>tailNumber</t>
   </si>
@@ -64,18 +64,22 @@
     <t>startUpLatitude</t>
   </si>
   <si>
-    <t>N672WM</t>
+    <t>N787QS</t>
   </si>
   <si>
-    <t>N2179L</t>
+    <t>N546XJ</t>
+  </si>
+  <si>
+    <t>N265SJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m\-d\-yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -118,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -133,6 +137,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -356,14 +366,14 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
@@ -430,13 +440,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="4">
-        <v>29.9917907714843</v>
+        <v>42.154861450195298</v>
       </c>
       <c r="C2" s="1">
-        <v>-95.291511535644503</v>
+        <v>-87.923774719238196</v>
       </c>
-      <c r="D2" s="3">
-        <v>42583</v>
+      <c r="D2" s="6">
+        <v>42583.851145833331</v>
       </c>
       <c r="E2" s="1">
         <v>29.9917907714843</v>
@@ -447,11 +457,11 @@
       <c r="G2" s="3">
         <v>42583</v>
       </c>
-      <c r="H2" s="1">
-        <v>29.9917907714843</v>
+      <c r="H2" s="4">
+        <v>42.154861450195298</v>
       </c>
-      <c r="I2" s="1">
-        <v>-95.291511535644503</v>
+      <c r="I2" s="4">
+        <v>-87.923774719238196</v>
       </c>
       <c r="J2" s="1">
         <v>2.2999999999999998</v>
@@ -482,13 +492,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="4">
-        <v>29.9917907714843</v>
+        <v>34.028289794921797</v>
       </c>
       <c r="C3" s="1">
-        <v>-95.291511535644503</v>
+        <v>-118.42420959472599</v>
       </c>
-      <c r="D3" s="3">
-        <v>42583</v>
+      <c r="D3" s="7">
+        <v>42583.812547928239</v>
       </c>
       <c r="E3" s="1">
         <v>29.9917907714843</v>
@@ -499,11 +509,11 @@
       <c r="G3" s="3">
         <v>42583</v>
       </c>
-      <c r="H3" s="1">
-        <v>29.9917907714843</v>
+      <c r="H3" s="4">
+        <v>34.028289794921797</v>
       </c>
-      <c r="I3" s="1">
-        <v>-95.291511535644503</v>
+      <c r="I3" s="4">
+        <v>-118.42420959472599</v>
       </c>
       <c r="J3" s="1">
         <v>2.2999999999999998</v>
@@ -530,18 +540,42 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>39.095008850097599</v>
+      </c>
+      <c r="C4" s="4">
+        <v>-84.422004699707003</v>
+      </c>
+      <c r="D4" s="7">
+        <v>42583.599294409723</v>
+      </c>
+      <c r="E4" s="4">
+        <v>29.9917907714843</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-95.291511535644503</v>
+      </c>
+      <c r="G4" s="3">
+        <v>42583</v>
+      </c>
+      <c r="H4" s="4">
+        <v>39.095008850097599</v>
+      </c>
+      <c r="I4" s="4">
+        <v>-84.422004699707003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>

</xml_diff>